<commit_message>
ERD ALL DAY EVERY DAY
</commit_message>
<xml_diff>
--- a/Database/Iteration 1 ERD Mapping.xlsx
+++ b/Database/Iteration 1 ERD Mapping.xlsx
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>